<commit_message>
Projects and gitignore added
</commit_message>
<xml_diff>
--- a/Projects/FitnessOnline/FitnessOnline_bug_reports.xlsx
+++ b/Projects/FitnessOnline/FitnessOnline_bug_reports.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Окружение</t>
+  </si>
+  <si>
+    <t>Вложения</t>
   </si>
   <si>
     <t>BR-1</t>
@@ -75,6 +78,9 @@
     <t>Смартфон Xiaomi Redmi Note 8 Pro, OS: Android 10.0, разрешение 2340*1080, диагональ 6,5'</t>
   </si>
   <si>
+    <t>Скринкаст</t>
+  </si>
+  <si>
     <t>BR-2</t>
   </si>
   <si>
@@ -169,6 +175,9 @@
     </r>
   </si>
   <si>
+    <t>Скриншот</t>
+  </si>
+  <si>
     <t>BR-5</t>
   </si>
   <si>
@@ -257,7 +266,7 @@
     <t>BR-6</t>
   </si>
   <si>
-    <t>В разделе Workouts на странице редактирования тренировочных дней значок в виде трех горизонтальных линий на плашке тренировкочного дня некликабелен</t>
+    <t>В разделе Workouts на странице редактирования тренировочных дней значок в виде трех горизонтальных линий на плашке тренировочного дня некликабелен</t>
   </si>
   <si>
     <r>
@@ -347,7 +356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -382,6 +391,10 @@
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -418,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -431,6 +444,9 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -438,6 +454,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -662,15 +681,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.63"/>
+    <col customWidth="1" min="1" max="1" width="5.88"/>
     <col customWidth="1" min="2" max="2" width="25.75"/>
-    <col customWidth="1" min="3" max="3" width="19.25"/>
-    <col customWidth="1" min="4" max="4" width="17.75"/>
+    <col customWidth="1" min="3" max="3" width="17.75"/>
+    <col customWidth="1" min="4" max="4" width="12.88"/>
     <col customWidth="1" min="5" max="5" width="25.5"/>
     <col customWidth="1" min="6" max="6" width="28.0"/>
-    <col customWidth="1" min="7" max="7" width="26.38"/>
-    <col customWidth="1" min="8" max="8" width="25.5"/>
-    <col customWidth="1" min="9" max="9" width="26.63"/>
+    <col customWidth="1" min="7" max="7" width="25.25"/>
+    <col customWidth="1" min="8" max="8" width="25.0"/>
+    <col customWidth="1" min="9" max="9" width="23.38"/>
+    <col customWidth="1" min="10" max="10" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -701,506 +721,530 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="I2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="J3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="H6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>17</v>
+      <c r="I8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -1211,6 +1255,15 @@
       <formula1>"Желательный,Стандартный,Критический,Блокирующий"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="J2"/>
+    <hyperlink r:id="rId2" ref="J3"/>
+    <hyperlink r:id="rId3" ref="J4"/>
+    <hyperlink r:id="rId4" ref="J5"/>
+    <hyperlink r:id="rId5" ref="J6"/>
+    <hyperlink r:id="rId6" ref="J7"/>
+    <hyperlink r:id="rId7" ref="J8"/>
+  </hyperlinks>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>